<commit_message>
Add new SVG and PNG assets for GUI; update Excel constants file
- Added SVG file for stop mode icon (om-2-stopMode-64x64-black.svg) to the operating mode GUI assets.
- Added PNG file for RFID graphic (rfid-36x30-nb-595257.png) to the PNG assets.
- Introduced a new version of the ADT constants Excel file (__ADT_CONSTANTS__-v1.0.xlsx) in the PLC library.
</commit_message>
<xml_diff>
--- a/PLC/90_Library/ADT/__ADT_CONSTANTS__-v1.1.xlsx
+++ b/PLC/90_Library/ADT/__ADT_CONSTANTS__-v1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.2\work\PlcFramework\PLC\90_Library\ADT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356DBC84-CC97-4576-8D90-3646AA870AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D1F96-C596-40A3-A1EC-FB2B682A39B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19215" yWindow="-16440" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -363,108 +363,6 @@
     <t xml:space="preserve"> Method 12: Read data from hash table </t>
   </si>
   <si>
-    <t>QUEUE_CMD_00_NIL</t>
-  </si>
-  <si>
-    <t>QUEUE_CMD_01_INIT</t>
-  </si>
-  <si>
-    <t>QUEUE_CMD_10_ENQUEUE</t>
-  </si>
-  <si>
-    <t>QUEUE_CMD_11_DEQUEUE</t>
-  </si>
-  <si>
-    <t>QUEUE_CMD_12_PEEK</t>
-  </si>
-  <si>
-    <t>STACK_CMD_00_NIL</t>
-  </si>
-  <si>
-    <t>STACK_CMD_01_INIT</t>
-  </si>
-  <si>
-    <t>STACK_CMD_10_PUSH</t>
-  </si>
-  <si>
-    <t>STACK_CMD_11_POP</t>
-  </si>
-  <si>
-    <t>STACK_CMD_12_PEEK</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_00_NIL</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_01_INIT</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_10_ADD_FIRST</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_11_ADD_LAST</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_12_ADD_INDEX</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_13_ADD_FIRST_HIGH_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_14_ADD_LAST_HIGH_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_15_ADD_FIRST_LOW_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_16_ADD_LAST_LOW_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_20_REMOVE_FIRST</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_21_REMOVE_LAST</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_22_REMOVE_INDEX</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_23_REMOVE_FIRST_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_24_REMOVE_LAST_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_30_READ_FIRST</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_31_READ_LAST</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_32_READ_INDEX</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_33_READ_FIRST_PRIORITY</t>
-  </si>
-  <si>
-    <t>LINKED_LIST_CMD_34_READ_LAST_PRIORITY</t>
-  </si>
-  <si>
-    <t>HASH_TABLE_CMD_00_NIL</t>
-  </si>
-  <si>
-    <t>HASH_TABLE_CMD_01_INIT</t>
-  </si>
-  <si>
-    <t>HASH_TABLE_CMD_10_ADD</t>
-  </si>
-  <si>
-    <t>HASH_TABLE_CMD_11_REMOVE</t>
-  </si>
-  <si>
-    <t>HASH_TABLE_CMD_12_READ</t>
-  </si>
-  <si>
     <t>STATUS_8033_FREE_SLOT_CORRUPTION</t>
   </si>
   <si>
@@ -472,6 +370,123 @@
   </si>
   <si>
     <t xml:space="preserve"> Status: Error - Free slot corruption</t>
+  </si>
+  <si>
+    <t>QUEUE_METHOD_00_NIL</t>
+  </si>
+  <si>
+    <t>QUEUE_METHOD_01_INIT</t>
+  </si>
+  <si>
+    <t>QUEUE_METHOD_10_ENQUEUE</t>
+  </si>
+  <si>
+    <t>QUEUE_METHOD_11_DEQUEUE</t>
+  </si>
+  <si>
+    <t>QUEUE_METHOD_12_PEEK</t>
+  </si>
+  <si>
+    <t>STACK_METHOD_00_NIL</t>
+  </si>
+  <si>
+    <t>STACK_METHOD_01_INIT</t>
+  </si>
+  <si>
+    <t>STACK_METHOD_10_PUSH</t>
+  </si>
+  <si>
+    <t>STACK_METHOD_11_POP</t>
+  </si>
+  <si>
+    <t>STACK_METHOD_12_PEEK</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_00_NIL</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_01_INIT</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_10_ADD_FIRST</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_11_ADD_LAST</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_12_ADD_INDEX</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_13_ADD_FIRST_HIGH_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_14_ADD_LAST_HIGH_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_15_ADD_FIRST_LOW_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_16_ADD_LAST_LOW_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_20_REMOVE_FIRST</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_21_REMOVE_LAST</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_22_REMOVE_INDEX</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_23_REMOVE_FIRST_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_24_REMOVE_LAST_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_30_READ_FIRST</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_31_READ_LAST</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_32_READ_INDEX</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_33_READ_FIRST_PRIORITY</t>
+  </si>
+  <si>
+    <t>LINKED_LIST_METHOD_34_READ_LAST_PRIORITY</t>
+  </si>
+  <si>
+    <t>HASH_TABLE_METHOD_00_NIL</t>
+  </si>
+  <si>
+    <t>HASH_TABLE_METHOD_01_INIT</t>
+  </si>
+  <si>
+    <t>HASH_TABLE_METHOD_10_ADD</t>
+  </si>
+  <si>
+    <t>HASH_TABLE_METHOD_11_REMOVE</t>
+  </si>
+  <si>
+    <t>HASH_TABLE_METHOD_12_READ</t>
+  </si>
+  <si>
+    <t>PRIORITY_QUEUE_METHOD_00_NIL</t>
+  </si>
+  <si>
+    <t>PRIORITY_QUEUE_METHOD_01_INIT</t>
+  </si>
+  <si>
+    <t>PRIORITY_QUEUE_METHOD_10_ENQUEUE</t>
+  </si>
+  <si>
+    <t>PRIORITY_QUEUE_METHOD_11_DEQUEUE</t>
+  </si>
+  <si>
+    <t>PRIORITY_QUEUE_METHOD_12_PEEK</t>
   </si>
 </sst>
 </file>
@@ -848,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1305,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1299,15 +1314,15 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -1324,7 +1339,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1341,7 +1356,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -1358,7 +1373,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -1375,7 +1390,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -1392,7 +1407,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -1409,7 +1424,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -1426,7 +1441,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1443,7 +1458,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -1460,7 +1475,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -1477,7 +1492,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -1494,7 +1509,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -1511,7 +1526,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -1523,12 +1538,12 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -1540,12 +1555,12 @@
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -1557,12 +1572,12 @@
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -1571,15 +1586,15 @@
         <v>9</v>
       </c>
       <c r="D42">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -1588,15 +1603,15 @@
         <v>9</v>
       </c>
       <c r="D43">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -1605,15 +1620,15 @@
         <v>9</v>
       </c>
       <c r="D44">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -1622,15 +1637,15 @@
         <v>9</v>
       </c>
       <c r="D45">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -1639,15 +1654,15 @@
         <v>9</v>
       </c>
       <c r="D46">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -1656,15 +1671,15 @@
         <v>9</v>
       </c>
       <c r="D47">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -1673,15 +1688,15 @@
         <v>9</v>
       </c>
       <c r="D48">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E48" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -1690,15 +1705,15 @@
         <v>9</v>
       </c>
       <c r="D49">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E49" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -1707,15 +1722,15 @@
         <v>9</v>
       </c>
       <c r="D50">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E50" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -1724,15 +1739,15 @@
         <v>9</v>
       </c>
       <c r="D51">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
@@ -1741,15 +1756,15 @@
         <v>9</v>
       </c>
       <c r="D52">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E52" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -1758,15 +1773,15 @@
         <v>9</v>
       </c>
       <c r="D53">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
@@ -1775,15 +1790,15 @@
         <v>9</v>
       </c>
       <c r="D54">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E54" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -1792,15 +1807,15 @@
         <v>9</v>
       </c>
       <c r="D55">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -1809,15 +1824,15 @@
         <v>9</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E56" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -1826,15 +1841,15 @@
         <v>9</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -1843,15 +1858,15 @@
         <v>9</v>
       </c>
       <c r="D58">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -1860,26 +1875,111 @@
         <v>9</v>
       </c>
       <c r="D59">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60">
+        <v>34</v>
+      </c>
+      <c r="E60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60">
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65">
         <v>12</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E65" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>